<commit_message>
Extra Stuff, needs to be continued...
</commit_message>
<xml_diff>
--- a/res/Development Log.xlsx
+++ b/res/Development Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandy\Source\repos\Programming Files - repos\Software Development\Coursework\ECM2414-Card-Game\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8991AB95-36EF-423A-92D7-493053034ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2677460-4C1F-4B0F-88E5-728EB33471F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{03E64FF8-3BC5-4669-B668-E0D7650BC561}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>Development Log</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Design &amp; Testing</t>
+  </si>
+  <si>
+    <t>Design &amp; Comments</t>
   </si>
 </sst>
 </file>
@@ -437,7 +440,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,12 +517,38 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="2">
+        <v>45620</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
+      <c r="B11" s="2">
+        <v>45621</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>

</xml_diff>